<commit_message>
update text label for graph
</commit_message>
<xml_diff>
--- a/data/Dictionary.xlsx
+++ b/data/Dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sopheap/Desktop/R/Microbiology Report 2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC11797-09D0-7649-A516-6E4E428FF9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2AC0C7-2B44-CD40-A373-A85D86160CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="1520" windowWidth="25600" windowHeight="15540" xr2:uid="{C15AEE32-6511-5147-A668-20441D5FEAF5}"/>
   </bookViews>
@@ -262,10 +262,10 @@
     <t>31-12-2022</t>
   </si>
   <si>
-    <t>Siem Reap Microbiology Team</t>
-  </si>
-  <si>
-    <t>Kampong Cham Provincial Referral Hospital</t>
+    <t>Battambang Microbiology Team</t>
+  </si>
+  <si>
+    <t>Siem Reap Provincial Referral Hospital</t>
   </si>
 </sst>
 </file>
@@ -733,7 +733,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
salmonella and bps from Jan to dec
</commit_message>
<xml_diff>
--- a/data/Dictionary.xlsx
+++ b/data/Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sopheap/Desktop/R/Microbiology Report 2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351A25D0-D95B-A84F-B354-65DCA34AB45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4A6DA0-DFD1-E041-AC6A-CE54DAC0B014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="1520" windowWidth="25600" windowHeight="15540" xr2:uid="{C15AEE32-6511-5147-A668-20441D5FEAF5}"/>
   </bookViews>
@@ -262,10 +262,10 @@
     <t>31-12-2022</t>
   </si>
   <si>
-    <t>Kampong Cham Provincial Referral Hospital</t>
-  </si>
-  <si>
-    <t>Kampong Cham Microbiology Team</t>
+    <t>Siem Reap Provincial Referral Hospital</t>
+  </si>
+  <si>
+    <t>Siem Reap Microbiology Team</t>
   </si>
 </sst>
 </file>
@@ -733,7 +733,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>